<commit_message>
banking time took me on a detour of looking at stage 4 again. Wrote functions to clean the lifebase and checkpoint cut off data really quickly
</commit_message>
<xml_diff>
--- a/TOR330 Data/4. TOR330 Timetable Data/TOR330_checkpoint_cut_offs_df.xlsx
+++ b/TOR330 Data/4. TOR330 Timetable Data/TOR330_checkpoint_cut_offs_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Checkpoint</t>
   </si>
@@ -22,13 +22,19 @@
     <t>Stage</t>
   </si>
   <si>
-    <t>distance_difference (km)</t>
-  </si>
-  <si>
-    <t>D+ difference (m)</t>
-  </si>
-  <si>
-    <t>Stage Duration</t>
+    <t>Checkpoint Distance (km)</t>
+  </si>
+  <si>
+    <t>Checkpoint Accumulated Distance Elevation (m)</t>
+  </si>
+  <si>
+    <t>Checkpoint Elevation Gain (m)</t>
+  </si>
+  <si>
+    <t>Checkpoint Accumulated Elevation (m)</t>
+  </si>
+  <si>
+    <t>Checkpoint Duration_seconds</t>
   </si>
   <si>
     <t>La Thuile</t>
@@ -55,12 +61,6 @@
     <t>Donnas OUT</t>
   </si>
   <si>
-    <t>Rifugio della Barma</t>
-  </si>
-  <si>
-    <t>Niel La Gruba</t>
-  </si>
-  <si>
     <t>Gressoney IN</t>
   </si>
   <si>
@@ -85,46 +85,40 @@
     <t>Ollomont OUT</t>
   </si>
   <si>
-    <t>FINISH</t>
-  </si>
-  <si>
-    <t>Stage 1</t>
+    <t>Stage1 Time</t>
   </si>
   <si>
     <t>Time Spent in Valgrisenche OUT</t>
   </si>
   <si>
-    <t>Stage 2</t>
+    <t>Stage2 Time</t>
   </si>
   <si>
     <t>Time Spent in Cogne OUT</t>
   </si>
   <si>
-    <t>Stage 3</t>
+    <t>Stage3 Time</t>
   </si>
   <si>
     <t>Time Spent in Donnas OUT</t>
   </si>
   <si>
-    <t>Stage 4</t>
+    <t>Stage4 Time</t>
   </si>
   <si>
     <t>Time Spent in Gressoney OUT</t>
   </si>
   <si>
-    <t>Stage 5</t>
+    <t>Stage5 Time</t>
   </si>
   <si>
     <t>Time Spent in Valtournenche OUT</t>
   </si>
   <si>
-    <t>Stage 6</t>
+    <t>Stage6 Time</t>
   </si>
   <si>
     <t>Time Spent in Ollomont OUT</t>
-  </si>
-  <si>
-    <t>Stage 7</t>
   </si>
 </sst>
 </file>
@@ -183,12 +177,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,13 +476,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,336 +498,376 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>18.98</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3">
-        <v>18.98</v>
+        <v>29.57</v>
       </c>
       <c r="D3">
-        <v>1602</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.2291666666666667</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>48.55</v>
+      </c>
+      <c r="E3">
+        <v>2737</v>
+      </c>
+      <c r="F3">
+        <v>4339</v>
+      </c>
+      <c r="G3">
+        <v>48600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
       </c>
       <c r="C4">
-        <v>29.57</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>2737</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.5625</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>48.55</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>4339</v>
+      </c>
+      <c r="G4">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>29.71000000000001</v>
       </c>
       <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.08333333333333333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>78.26000000000001</v>
+      </c>
+      <c r="E5">
+        <v>2835</v>
+      </c>
+      <c r="F5">
+        <v>7174</v>
+      </c>
+      <c r="G5">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6">
-        <v>29.71000000000001</v>
+        <v>25.73999999999999</v>
       </c>
       <c r="D6">
-        <v>2835</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.5208333333333334</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>104</v>
+      </c>
+      <c r="E6">
+        <v>2108</v>
+      </c>
+      <c r="F6">
+        <v>9282</v>
+      </c>
+      <c r="G6">
+        <v>30600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
       </c>
       <c r="C7">
-        <v>25.73999999999999</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>2108</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.3541666666666667</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>104</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>9282</v>
+      </c>
+      <c r="G7">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>45.77000000000001</v>
       </c>
       <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.08333333333333333</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>149.77</v>
+      </c>
+      <c r="E8">
+        <v>2768</v>
+      </c>
+      <c r="F8">
+        <v>12050</v>
+      </c>
+      <c r="G8">
+        <v>64800.00000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>28</v>
       </c>
       <c r="C9">
-        <v>45.77000000000001</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>2768</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>149.77</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>12050</v>
+      </c>
+      <c r="G9">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>29</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>54.22999999999999</v>
       </c>
       <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.08333333333333333</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>204</v>
+      </c>
+      <c r="E10">
+        <v>5933</v>
+      </c>
+      <c r="F10">
+        <v>17983</v>
+      </c>
+      <c r="G10">
+        <v>75600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
       </c>
       <c r="C11">
-        <v>26.01999999999998</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>3462</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.4583333333333333</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>204</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>17983</v>
+      </c>
+      <c r="G11">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12">
-        <v>14.89000000000001</v>
+        <v>16.97999999999999</v>
       </c>
       <c r="D12">
-        <v>1477</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.2708333333333333</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>220.98</v>
+      </c>
+      <c r="E12">
+        <v>1691</v>
+      </c>
+      <c r="F12">
+        <v>19674</v>
+      </c>
+      <c r="G12">
+        <v>43200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13">
-        <v>13.31999999999999</v>
+        <v>16.64000000000001</v>
       </c>
       <c r="D13">
-        <v>994</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.1458333333333333</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>237.62</v>
+      </c>
+      <c r="E13">
+        <v>1403</v>
+      </c>
+      <c r="F13">
+        <v>21077</v>
+      </c>
+      <c r="G13">
+        <v>21600</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.08333333333333333</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>237.62</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>21077</v>
+      </c>
+      <c r="G14">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15">
-        <v>16.97999999999999</v>
+        <v>36.18000000000001</v>
       </c>
       <c r="D15">
-        <v>1691</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>273.8</v>
+      </c>
+      <c r="E15">
+        <v>3206</v>
+      </c>
+      <c r="F15">
+        <v>24283</v>
+      </c>
+      <c r="G15">
+        <v>54000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16">
-        <v>16.64000000000001</v>
+        <v>11.86000000000001</v>
       </c>
       <c r="D16">
-        <v>1403</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>285.66</v>
+      </c>
+      <c r="E16">
+        <v>1419</v>
+      </c>
+      <c r="F16">
+        <v>25702</v>
+      </c>
+      <c r="G16">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.08333333333333333</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18">
-        <v>36.18000000000001</v>
-      </c>
-      <c r="D18">
-        <v>3206</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19">
-        <v>11.86000000000001</v>
-      </c>
-      <c r="D19">
-        <v>1419</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.2083333333333333</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0.08333333333333333</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21">
-        <v>49.65999999999997</v>
-      </c>
-      <c r="D21">
-        <v>3906</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0.875</v>
+        <v>285.66</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>25702</v>
+      </c>
+      <c r="G17">
+        <v>7200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIxing cut off issues and stage 6
</commit_message>
<xml_diff>
--- a/TOR330 Data/4. TOR330 Timetable Data/TOR330_checkpoint_cut_offs_df.xlsx
+++ b/TOR330 Data/4. TOR330 Timetable Data/TOR330_checkpoint_cut_offs_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Checkpoint</t>
   </si>
@@ -37,6 +37,9 @@
     <t>Checkpoint Duration_seconds</t>
   </si>
   <si>
+    <t>Running Total Checkpoint Duration_seconds</t>
+  </si>
+  <si>
     <t>La Thuile</t>
   </si>
   <si>
@@ -46,7 +49,7 @@
     <t>Valgrisenche OUT</t>
   </si>
   <si>
-    <t>Eaux Rousses</t>
+    <t>Eaux Rousse</t>
   </si>
   <si>
     <t>Cogne IN</t>
@@ -61,6 +64,12 @@
     <t>Donnas OUT</t>
   </si>
   <si>
+    <t>Rifugio della Barma</t>
+  </si>
+  <si>
+    <t>Niel La Gruba</t>
+  </si>
+  <si>
     <t>Gressoney IN</t>
   </si>
   <si>
@@ -85,40 +94,46 @@
     <t>Ollomont OUT</t>
   </si>
   <si>
-    <t>Stage1 Time</t>
-  </si>
-  <si>
-    <t>Time Spent in Valgrisenche OUT</t>
-  </si>
-  <si>
-    <t>Stage2 Time</t>
-  </si>
-  <si>
-    <t>Time Spent in Cogne OUT</t>
-  </si>
-  <si>
-    <t>Stage3 Time</t>
-  </si>
-  <si>
-    <t>Time Spent in Donnas OUT</t>
-  </si>
-  <si>
-    <t>Stage4 Time</t>
-  </si>
-  <si>
-    <t>Time Spent in Gressoney OUT</t>
-  </si>
-  <si>
-    <t>Stage5 Time</t>
-  </si>
-  <si>
-    <t>Time Spent in Valtournenche OUT</t>
-  </si>
-  <si>
-    <t>Stage6 Time</t>
-  </si>
-  <si>
-    <t>Time Spent in Ollomont OUT</t>
+    <t>FINISH</t>
+  </si>
+  <si>
+    <t>Stage 1</t>
+  </si>
+  <si>
+    <t>Time Spent in Valgrisenche</t>
+  </si>
+  <si>
+    <t>Stage 2</t>
+  </si>
+  <si>
+    <t>Time Spent in Cogne</t>
+  </si>
+  <si>
+    <t>Stage 3</t>
+  </si>
+  <si>
+    <t>Time Spent in Donnas</t>
+  </si>
+  <si>
+    <t>Stage 4</t>
+  </si>
+  <si>
+    <t>Time Spent in Gressoney</t>
+  </si>
+  <si>
+    <t>Stage 5</t>
+  </si>
+  <si>
+    <t>Time Spent in Valtournenche</t>
+  </si>
+  <si>
+    <t>Stage 6</t>
+  </si>
+  <si>
+    <t>Time Spent in Ollomont</t>
+  </si>
+  <si>
+    <t>Stage 7</t>
   </si>
 </sst>
 </file>
@@ -476,13 +491,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,33 +519,42 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>18.98</v>
       </c>
       <c r="D2">
         <v>18.98</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1602</v>
       </c>
       <c r="F2">
         <v>1602</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="G2">
+        <v>19800</v>
+      </c>
+      <c r="H2">
+        <v>19800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>29.57</v>
@@ -547,13 +571,16 @@
       <c r="G3">
         <v>48600</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <v>68400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -570,13 +597,16 @@
       <c r="G4">
         <v>7200</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <v>75600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>29.71000000000001</v>
@@ -593,13 +623,16 @@
       <c r="G5">
         <v>45000</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <v>120600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>25.73999999999999</v>
@@ -616,13 +649,16 @@
       <c r="G6">
         <v>30600</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6">
+        <v>151200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -639,13 +675,16 @@
       <c r="G7">
         <v>7200</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7">
+        <v>158400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C8">
         <v>45.77000000000001</v>
@@ -662,13 +701,16 @@
       <c r="G8">
         <v>64800.00000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8">
+        <v>223200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -685,189 +727,294 @@
       <c r="G9">
         <v>7200</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9">
+        <v>230400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C10">
-        <v>54.22999999999999</v>
+        <v>26.01999999999998</v>
       </c>
       <c r="D10">
+        <v>175.79</v>
+      </c>
+      <c r="E10">
+        <v>3462</v>
+      </c>
+      <c r="F10">
+        <v>15512</v>
+      </c>
+      <c r="G10">
+        <v>39600</v>
+      </c>
+      <c r="H10">
+        <v>270000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11">
+        <v>14.89000000000001</v>
+      </c>
+      <c r="D11">
+        <v>190.68</v>
+      </c>
+      <c r="E11">
+        <v>1477</v>
+      </c>
+      <c r="F11">
+        <v>16989</v>
+      </c>
+      <c r="G11">
+        <v>23400</v>
+      </c>
+      <c r="H11">
+        <v>293400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12">
+        <v>13.31999999999999</v>
+      </c>
+      <c r="D12">
         <v>204</v>
       </c>
-      <c r="E10">
-        <v>5933</v>
-      </c>
-      <c r="F10">
+      <c r="E12">
+        <v>994</v>
+      </c>
+      <c r="F12">
         <v>17983</v>
       </c>
-      <c r="G10">
+      <c r="G12">
+        <v>12600</v>
+      </c>
+      <c r="H12">
+        <v>306000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>204</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>17983</v>
+      </c>
+      <c r="G13">
+        <v>7200</v>
+      </c>
+      <c r="H13">
+        <v>313200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <v>16.97999999999999</v>
+      </c>
+      <c r="D14">
+        <v>220.98</v>
+      </c>
+      <c r="E14">
+        <v>1691</v>
+      </c>
+      <c r="F14">
+        <v>19674</v>
+      </c>
+      <c r="G14">
+        <v>43200</v>
+      </c>
+      <c r="H14">
+        <v>356400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15">
+        <v>16.64000000000001</v>
+      </c>
+      <c r="D15">
+        <v>237.62</v>
+      </c>
+      <c r="E15">
+        <v>1403</v>
+      </c>
+      <c r="F15">
+        <v>21077</v>
+      </c>
+      <c r="G15">
+        <v>21600</v>
+      </c>
+      <c r="H15">
+        <v>378000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>237.62</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>21077</v>
+      </c>
+      <c r="G16">
+        <v>7200</v>
+      </c>
+      <c r="H16">
+        <v>385200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17">
+        <v>36.18000000000001</v>
+      </c>
+      <c r="D17">
+        <v>273.8</v>
+      </c>
+      <c r="E17">
+        <v>3206</v>
+      </c>
+      <c r="F17">
+        <v>24283</v>
+      </c>
+      <c r="G17">
+        <v>54000</v>
+      </c>
+      <c r="H17">
+        <v>439200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18">
+        <v>11.86000000000001</v>
+      </c>
+      <c r="D18">
+        <v>285.66</v>
+      </c>
+      <c r="E18">
+        <v>1419</v>
+      </c>
+      <c r="F18">
+        <v>25702</v>
+      </c>
+      <c r="G18">
+        <v>18000</v>
+      </c>
+      <c r="H18">
+        <v>457200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>285.66</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>25702</v>
+      </c>
+      <c r="G19">
+        <v>7200</v>
+      </c>
+      <c r="H19">
+        <v>464400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20">
+        <v>49.65999999999997</v>
+      </c>
+      <c r="D20">
+        <v>335.32</v>
+      </c>
+      <c r="E20">
+        <v>3906</v>
+      </c>
+      <c r="F20">
+        <v>29608</v>
+      </c>
+      <c r="G20">
         <v>75600</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>204</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>17983</v>
-      </c>
-      <c r="G11">
-        <v>7200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12">
-        <v>16.97999999999999</v>
-      </c>
-      <c r="D12">
-        <v>220.98</v>
-      </c>
-      <c r="E12">
-        <v>1691</v>
-      </c>
-      <c r="F12">
-        <v>19674</v>
-      </c>
-      <c r="G12">
-        <v>43200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13">
-        <v>16.64000000000001</v>
-      </c>
-      <c r="D13">
-        <v>237.62</v>
-      </c>
-      <c r="E13">
-        <v>1403</v>
-      </c>
-      <c r="F13">
-        <v>21077</v>
-      </c>
-      <c r="G13">
-        <v>21600</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>237.62</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>21077</v>
-      </c>
-      <c r="G14">
-        <v>7200</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15">
-        <v>36.18000000000001</v>
-      </c>
-      <c r="D15">
-        <v>273.8</v>
-      </c>
-      <c r="E15">
-        <v>3206</v>
-      </c>
-      <c r="F15">
-        <v>24283</v>
-      </c>
-      <c r="G15">
-        <v>54000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16">
-        <v>11.86000000000001</v>
-      </c>
-      <c r="D16">
-        <v>285.66</v>
-      </c>
-      <c r="E16">
-        <v>1419</v>
-      </c>
-      <c r="F16">
-        <v>25702</v>
-      </c>
-      <c r="G16">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>285.66</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>25702</v>
-      </c>
-      <c r="G17">
-        <v>7200</v>
+      <c r="H20">
+        <v>540000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>